<commit_message>
Added Android Development stages
</commit_message>
<xml_diff>
--- a/Rough Plan.xlsx
+++ b/Rough Plan.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Rough breakdown of project</t>
   </si>
@@ -34,6 +34,36 @@
   </si>
   <si>
     <t>Planning and Design</t>
+  </si>
+  <si>
+    <t>Description of system</t>
+  </si>
+  <si>
+    <t>Use Case Diagram</t>
+  </si>
+  <si>
+    <t>Class Diagrams</t>
+  </si>
+  <si>
+    <t>Database design</t>
+  </si>
+  <si>
+    <t>Screen Design</t>
+  </si>
+  <si>
+    <t>Module to convert file (xml) to Form screen</t>
+  </si>
+  <si>
+    <t>Create Android database or some other form of store</t>
+  </si>
+  <si>
+    <t>Module to receive form schema</t>
+  </si>
+  <si>
+    <t>Module to send completed form data</t>
+  </si>
+  <si>
+    <t>User interface</t>
   </si>
 </sst>
 </file>
@@ -374,16 +404,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -408,8 +438,46 @@
       </c>
     </row>
     <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
       <c r="B3" t="s">
         <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed draft 1 of rough plan
</commit_message>
<xml_diff>
--- a/Rough Plan.xlsx
+++ b/Rough Plan.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Rough breakdown of project</t>
   </si>
@@ -54,9 +54,6 @@
     <t>Module to convert file (xml) to Form screen</t>
   </si>
   <si>
-    <t>Create Android database or some other form of store</t>
-  </si>
-  <si>
     <t>Module to receive form schema</t>
   </si>
   <si>
@@ -64,6 +61,36 @@
   </si>
   <si>
     <t>User interface</t>
+  </si>
+  <si>
+    <t>module to create form schema</t>
+  </si>
+  <si>
+    <t>Form schema design</t>
+  </si>
+  <si>
+    <t>Module to receive completed form data</t>
+  </si>
+  <si>
+    <t>Module to create Android database or some other form of store</t>
+  </si>
+  <si>
+    <t>Module to store completed form data</t>
+  </si>
+  <si>
+    <t>Module to query data</t>
+  </si>
+  <si>
+    <t>Design any necessary protocols</t>
+  </si>
+  <si>
+    <t>create module for sending out form schemas</t>
+  </si>
+  <si>
+    <t>Design security</t>
+  </si>
+  <si>
+    <t>Create databases.</t>
   </si>
 </sst>
 </file>
@@ -404,17 +431,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="49" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -445,7 +472,10 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -455,13 +485,25 @@
       <c r="B4" t="s">
         <v>11</v>
       </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -469,7 +511,10 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -477,7 +522,18 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified Project Plan Gaant chart
</commit_message>
<xml_diff>
--- a/Rough Plan.xlsx
+++ b/Rough Plan.xlsx
@@ -433,8 +433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>